<commit_message>
initial victory implement, initial scoring system, initial gameflow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D648C54-3975-4CD6-8ED8-D1BF12EA0B61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="1050" windowWidth="21600" windowHeight="12345"/>
+    <workbookView xWindow="2055" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Key</t>
   </si>
@@ -43,12 +44,24 @@
   </si>
   <si>
     <t>Math Multiplication</t>
+  </si>
+  <si>
+    <t>multiply</t>
+  </si>
+  <si>
+    <t>divide</t>
+  </si>
+  <si>
+    <t>Multiply</t>
+  </si>
+  <si>
+    <t>Divide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,11 +387,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,6 +438,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
victory modal, more background stuff, some tweaks
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D582F46-6D43-4AA6-9F86-D1014DACFEA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11947986-63FE-4A37-929C-608C8A394344}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2055" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Key</t>
   </si>
@@ -74,6 +74,42 @@
   </si>
   <si>
     <t>GO</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>time_bonus</t>
+  </si>
+  <si>
+    <t>TIME BONUS</t>
+  </si>
+  <si>
+    <t>perfect</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>PERFECT</t>
   </si>
 </sst>
 </file>
@@ -406,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +532,54 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added options modal, some adjustment on how palette is handled
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11947986-63FE-4A37-929C-608C8A394344}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBE48DA-85E6-4CE6-8E10-0A8C478CA464}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2055" yWindow="2385" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Key</t>
   </si>
@@ -110,6 +110,48 @@
   </si>
   <si>
     <t>PERFECT</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>OPTIONS</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>sound</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>speech</t>
+  </si>
+  <si>
+    <t>SPEECH</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>CLOSE</t>
   </si>
 </sst>
 </file>
@@ -442,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,6 +622,62 @@
         <v>28</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
some lesson 2 preps
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E83B54-7393-41E3-9A18-111B254BECB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3462D61-8B4D-48E1-A426-349D9D6236D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="3405" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>Key</t>
   </si>
@@ -154,12 +154,6 @@
     <t>CLOSE</t>
   </si>
   <si>
-    <t>tutorialOpExample1</t>
-  </si>
-  <si>
-    <t>2 x 3 = 6\n3 x 2 = 6</t>
-  </si>
-  <si>
     <t>lesson_1_intro_1</t>
   </si>
   <si>
@@ -169,15 +163,9 @@
     <t>lesson_1_mult2_1</t>
   </si>
   <si>
-    <t>In multiples of two, the trick is to simply add the number by itself.</t>
-  </si>
-  <si>
     <t>lesson_1_mult2_2</t>
   </si>
   <si>
-    <t>lesson_1_mult2_3</t>
-  </si>
-  <si>
     <t>mult2_title</t>
   </si>
   <si>
@@ -205,25 +193,142 @@
     <t>lesson_1_tutorial_end_1</t>
   </si>
   <si>
-    <t>Now banish these blobs by connecting them in the correct order.</t>
-  </si>
-  <si>
     <t>Excellent! You are now ready for the mission!</t>
   </si>
   <si>
     <t>The commutative property means that multiplying numbers in any order gives the same answer.</t>
   </si>
   <si>
-    <t>That's all there is to it with multiples of 2.</t>
-  </si>
-  <si>
-    <t>For example: 2 times 3, and 3 times 2, equal 6.</t>
-  </si>
-  <si>
-    <t>For example: 2 times 6 can be seen as 6 plus 6, which equals to 12.</t>
-  </si>
-  <si>
     <t>With this trick, you only have to remember half the multiplication table!</t>
+  </si>
+  <si>
+    <t>lesson_2_mult3_1</t>
+  </si>
+  <si>
+    <t>In multiples of two, the trick is to simply double the number.</t>
+  </si>
+  <si>
+    <t>In multiples of three: double the number, and then add the original number.</t>
+  </si>
+  <si>
+    <t>lesson_2_mult3_2</t>
+  </si>
+  <si>
+    <t>lesson_2_mult4_1</t>
+  </si>
+  <si>
+    <t>In multiples of four: double the number, and then double it again.</t>
+  </si>
+  <si>
+    <t>lesson_2_mult4_2</t>
+  </si>
+  <si>
+    <t>lesson_2_div_1</t>
+  </si>
+  <si>
+    <t>For example: 2 x 6 can be 6 + 6, which equals to 12.</t>
+  </si>
+  <si>
+    <t>For example: 2 x 3, and 3 x 2, equal 6.</t>
+  </si>
+  <si>
+    <t>For example: 3 x 6 can be expressed as (6 x 2) + 6, which becomes 12 + 6, giving you 18.</t>
+  </si>
+  <si>
+    <t>lesson_2_div_2</t>
+  </si>
+  <si>
+    <t>When it comes to division, think of it as the opposite of multiplication.</t>
+  </si>
+  <si>
+    <t>lesson_2_div_3</t>
+  </si>
+  <si>
+    <t>lesson_2_tutorial_1</t>
+  </si>
+  <si>
+    <t>Now banish these blobs by connecting them in the correct order using multiplication.</t>
+  </si>
+  <si>
+    <t>Now banish these blobs by connecting them in the correct order using division.</t>
+  </si>
+  <si>
+    <t>lesson_2_div_4</t>
+  </si>
+  <si>
+    <t>Unlike multiplication, division is not commutative. So the order of the numbers cannot be changed.</t>
+  </si>
+  <si>
+    <t>Rearranging the equation, and replacing division with multiplication can help.</t>
+  </si>
+  <si>
+    <t>lesson_2_tutorial_end_1</t>
+  </si>
+  <si>
+    <t>mult3_title</t>
+  </si>
+  <si>
+    <t>mult4_title</t>
+  </si>
+  <si>
+    <t>mult5_title</t>
+  </si>
+  <si>
+    <t>mult6_title</t>
+  </si>
+  <si>
+    <t>mult7_title</t>
+  </si>
+  <si>
+    <t>mult8_title</t>
+  </si>
+  <si>
+    <t>mult9_title</t>
+  </si>
+  <si>
+    <t>mult10_title</t>
+  </si>
+  <si>
+    <t>Multiples of 3</t>
+  </si>
+  <si>
+    <t>Multiples of 4</t>
+  </si>
+  <si>
+    <t>Multiples of 5</t>
+  </si>
+  <si>
+    <t>Multiples of 6</t>
+  </si>
+  <si>
+    <t>Multiples of 7</t>
+  </si>
+  <si>
+    <t>Multiples of 8</t>
+  </si>
+  <si>
+    <t>Multiples of 9</t>
+  </si>
+  <si>
+    <t>Multiples of 10</t>
+  </si>
+  <si>
+    <t>For example: 4 x 6, double 6 to get 12, and then double 12 to get 24.</t>
+  </si>
+  <si>
+    <t>division</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>For example: 21 ÷ 3 = ? can be rearranged to ? x 3 = 21. From here, we can deduce that 7 x 3 = 21.</t>
+  </si>
+  <si>
+    <t>not_commutative</t>
+  </si>
+  <si>
+    <t>Not Commutative!</t>
   </si>
 </sst>
 </file>
@@ -556,9 +661,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -752,98 +857,242 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>60</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B42" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>67</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added mult table modal, some lesson tweaks, prep lesson 3
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3462D61-8B4D-48E1-A426-349D9D6236D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{533683F6-60B5-443B-AC68-94F2E2730B57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
   <si>
     <t>Key</t>
   </si>
@@ -157,9 +157,6 @@
     <t>lesson_1_intro_1</t>
   </si>
   <si>
-    <t>Before we begin our mission, let's first learn about some tricks with multiplication!</t>
-  </si>
-  <si>
     <t>lesson_1_mult2_1</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>For example: 2 x 3, and 3 x 2, equal 6.</t>
   </si>
   <si>
-    <t>For example: 3 x 6 can be expressed as (6 x 2) + 6, which becomes 12 + 6, giving you 18.</t>
-  </si>
-  <si>
     <t>lesson_2_div_2</t>
   </si>
   <si>
@@ -250,12 +244,6 @@
     <t>Now banish these blobs by connecting them in the correct order using multiplication.</t>
   </si>
   <si>
-    <t>Now banish these blobs by connecting them in the correct order using division.</t>
-  </si>
-  <si>
-    <t>lesson_2_div_4</t>
-  </si>
-  <si>
     <t>Unlike multiplication, division is not commutative. So the order of the numbers cannot be changed.</t>
   </si>
   <si>
@@ -322,13 +310,49 @@
     <t>Division</t>
   </si>
   <si>
-    <t>For example: 21 ÷ 3 = ? can be rearranged to ? x 3 = 21. From here, we can deduce that 7 x 3 = 21.</t>
-  </si>
-  <si>
     <t>not_commutative</t>
   </si>
   <si>
     <t>Not Commutative!</t>
+  </si>
+  <si>
+    <t>lesson_2_intro_1</t>
+  </si>
+  <si>
+    <t>Good work! Now it's time to step up the game with multiples of 3 and 4.</t>
+  </si>
+  <si>
+    <t>lesson_2_intro_2</t>
+  </si>
+  <si>
+    <t>Let me show you some neat tricks.</t>
+  </si>
+  <si>
+    <t>For the next mission, some blobs must be matched with division. Go ahead and try it out.</t>
+  </si>
+  <si>
+    <t>multiplicationTable</t>
+  </si>
+  <si>
+    <t>Multiplication Table</t>
+  </si>
+  <si>
+    <t>multTable_instruct</t>
+  </si>
+  <si>
+    <t>Press this button to review the multiplication table.</t>
+  </si>
+  <si>
+    <t>Press this button to proceed.</t>
+  </si>
+  <si>
+    <t>proceed_instruct</t>
+  </si>
+  <si>
+    <t>Before we proceed, let's first learn some tricks with multiplication!</t>
+  </si>
+  <si>
+    <t>For example: 3 x 6, double 6 to get 12, and then add 6 to get 18.</t>
   </si>
 </sst>
 </file>
@@ -661,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -823,7 +847,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -831,7 +855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -839,7 +863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -847,7 +871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -855,244 +879,282 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>84</v>
-      </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>98</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B45" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
         <v>101</v>
       </c>
-      <c r="B33" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>55</v>
-      </c>
-      <c r="B40" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>73</v>
-      </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gameflow stuff, start art/animation
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDD9DC8-823C-41F4-A9ED-102F152FB56F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FBE96F-A6B4-4820-B1D4-8DD5BA159FFA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="3750" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
   <si>
     <t>Key</t>
   </si>
@@ -43,9 +43,6 @@
     <t>title</t>
   </si>
   <si>
-    <t>Math Multiplication</t>
-  </si>
-  <si>
     <t>multiply</t>
   </si>
   <si>
@@ -545,6 +542,33 @@
   </si>
   <si>
     <t>...also 100, 1000, and so forth.</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>COMPLETE</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>PLAY</t>
+  </si>
+  <si>
+    <t>&lt;size=50&gt;Attack on Blob&lt;/size&gt;\nMultiply and Divide</t>
+  </si>
+  <si>
+    <t>credits</t>
+  </si>
+  <si>
+    <t>credits_desc</t>
+  </si>
+  <si>
+    <t>Written by: David Dionisio\nMusic from: Kevin Macleod</t>
+  </si>
+  <si>
+    <t>CREDITS</t>
   </si>
 </sst>
 </file>
@@ -594,9 +618,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -877,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,387 +950,387 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
+        <v>179</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
+        <v>180</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>174</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33">
-        <v>5</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>172</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>155</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>102</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>103</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>151</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>56</v>
@@ -1311,298 +1338,330 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>114</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B68" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B69" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B70" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B71" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B72" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B73" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B77" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B79" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B81" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="B85" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>162</v>
+      </c>
+      <c r="B87" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>165</v>
+      </c>
+      <c r="B89" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>169</v>
+      </c>
+      <c r="B91" t="s">
         <v>170</v>
-      </c>
-      <c r="B87" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaks, bug fixes, submit stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C2365C-2E94-4E81-AA9E-AE81948C8A56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E423AC6-017E-4D93-9B9B-F288990F82D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3630" yWindow="3915" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="215">
   <si>
     <t>Key</t>
   </si>
@@ -232,9 +232,6 @@
     <t>Now banish these blobs by connecting them in the correct order using multiplication.</t>
   </si>
   <si>
-    <t>Unlike multiplication, division is not commutative. So the order of the numbers cannot be changed.</t>
-  </si>
-  <si>
     <t>Rearranging the equation, and replacing division with multiplication can help.</t>
   </si>
   <si>
@@ -304,12 +301,6 @@
     <t>lesson_2_intro_1</t>
   </si>
   <si>
-    <t>lesson_2_intro_2</t>
-  </si>
-  <si>
-    <t>Let me show you some neat tricks.</t>
-  </si>
-  <si>
     <t>For the next mission, some blobs must be matched with division. Go ahead and try it out.</t>
   </si>
   <si>
@@ -658,9 +649,6 @@
     <t>congrats_desc</t>
   </si>
   <si>
-    <t>You have banished all the blobs! Earth is safe once more!</t>
-  </si>
-  <si>
     <t>Thank you for playing!</t>
   </si>
   <si>
@@ -671,6 +659,12 @@
   </si>
   <si>
     <t>We must strike them down!</t>
+  </si>
+  <si>
+    <t>Unlike multiplication, division is not commutative. So, the order of the numbers cannot be changed.</t>
+  </si>
+  <si>
+    <t>You have banished all the blobs! Earth is safe!</t>
   </si>
 </sst>
 </file>
@@ -1006,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,31 +1047,31 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1098,18 +1092,18 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,66 +1236,66 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
         <v>189</v>
-      </c>
-      <c r="B33" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B34" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1314,128 +1308,128 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" t="s">
         <v>89</v>
-      </c>
-      <c r="B49" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1448,34 +1442,34 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B52" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B53" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s">
         <v>91</v>
-      </c>
-      <c r="B54" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1483,7 +1477,7 @@
         <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1501,7 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1536,90 +1530,90 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B64" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1627,95 +1621,95 @@
         <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>107</v>
+      </c>
+      <c r="B76" t="s">
         <v>108</v>
-      </c>
-      <c r="B76" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B79" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>113</v>
+      </c>
+      <c r="B80" t="s">
         <v>114</v>
-      </c>
-      <c r="B80" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>115</v>
+      </c>
+      <c r="B81" t="s">
         <v>116</v>
-      </c>
-      <c r="B81" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>117</v>
+      </c>
+      <c r="B82" t="s">
         <v>118</v>
-      </c>
-      <c r="B82" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>119</v>
+      </c>
+      <c r="B83" t="s">
         <v>120</v>
-      </c>
-      <c r="B83" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B84" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1723,63 +1717,63 @@
         <v>134</v>
       </c>
       <c r="B86" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B87" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>137</v>
+      </c>
+      <c r="B88" t="s">
         <v>138</v>
-      </c>
-      <c r="B88" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B89" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B90" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B91" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B93" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1787,128 +1781,120 @@
         <v>157</v>
       </c>
       <c r="B94" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B95" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B96" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>162</v>
+      </c>
+      <c r="B97" t="s">
         <v>163</v>
-      </c>
-      <c r="B97" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" t="s">
         <v>165</v>
-      </c>
-      <c r="B98" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="B99" t="s">
-        <v>168</v>
+        <v>207</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B100" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="C100">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B101" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C101">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B102" t="s">
-        <v>213</v>
-      </c>
-      <c r="C102">
-        <v>3</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>196</v>
+      </c>
+      <c r="B103" t="s">
         <v>197</v>
-      </c>
-      <c r="B103" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>198</v>
+      </c>
+      <c r="B104" t="s">
         <v>199</v>
-      </c>
-      <c r="B104" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>200</v>
+      </c>
+      <c r="B105" t="s">
         <v>201</v>
-      </c>
-      <c r="B105" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>202</v>
+      </c>
+      <c r="B106" t="s">
         <v>203</v>
-      </c>
-      <c r="B106" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>204</v>
+      </c>
+      <c r="B107" t="s">
         <v>205</v>
-      </c>
-      <c r="B107" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>207</v>
-      </c>
-      <c r="B108" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected texts, updated project to latest unity
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E423AC6-017E-4D93-9B9B-F288990F82D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA8E56-265D-4147-99DA-F189D626AF26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="3915" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -190,18 +190,12 @@
     <t>The commutative property means that multiplying numbers in any order gives the same answer.</t>
   </si>
   <si>
-    <t>With this trick, you only have to remember half the multiplication table!</t>
-  </si>
-  <si>
     <t>lesson_2_mult3_1</t>
   </si>
   <si>
     <t>In multiples of two, the trick is to simply double the number.</t>
   </si>
   <si>
-    <t>In multiples of three: double the number, and then add the original number.</t>
-  </si>
-  <si>
     <t>lesson_2_mult3_2</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>Now banish these blobs by connecting them in the correct order using multiplication.</t>
   </si>
   <si>
-    <t>Rearranging the equation, and replacing division with multiplication can help.</t>
-  </si>
-  <si>
     <t>lesson_2_tutorial_end_1</t>
   </si>
   <si>
@@ -301,9 +292,6 @@
     <t>lesson_2_intro_1</t>
   </si>
   <si>
-    <t>For the next mission, some blobs must be matched with division. Go ahead and try it out.</t>
-  </si>
-  <si>
     <t>multiplicationTable</t>
   </si>
   <si>
@@ -322,9 +310,6 @@
     <t>proceed_instruct</t>
   </si>
   <si>
-    <t>Before we proceed, let's first learn some tricks with multiplication!</t>
-  </si>
-  <si>
     <t>lesson_3_intro_1</t>
   </si>
   <si>
@@ -391,18 +376,6 @@
     <t>Associative Property</t>
   </si>
   <si>
-    <t>For example: 2 x 3 and 3 x 2 equal 6.</t>
-  </si>
-  <si>
-    <t>For example, 3 x 6: double 6 to get 12, and then add 6 to get 18.</t>
-  </si>
-  <si>
-    <t>For example, 4 x 6: double 6 to get 12, and then double 12 to get 24.</t>
-  </si>
-  <si>
-    <t>For example, 6 x 7: multiply 7 by 5 to get 35, and then add 7 to get 42.</t>
-  </si>
-  <si>
     <t>not_associative</t>
   </si>
   <si>
@@ -436,9 +409,6 @@
     <t>lesson_4_mult8_2</t>
   </si>
   <si>
-    <t>For example, 8 x 4: double 4 to get 8, double 8 to get 16, and finally double 16 to get 32.</t>
-  </si>
-  <si>
     <t>lesson_4_distributive_1</t>
   </si>
   <si>
@@ -451,9 +421,6 @@
     <t>lesson_4_end_1</t>
   </si>
   <si>
-    <t>Now onwards to the next mission!</t>
-  </si>
-  <si>
     <t>distributive_title</t>
   </si>
   <si>
@@ -478,9 +445,6 @@
     <t>The distributive property allows you to distribute a number to a group.</t>
   </si>
   <si>
-    <t>For multiplication, this is a good trick for splitting up a number, and computing each one separately.</t>
-  </si>
-  <si>
     <t>As they say: when an obstacle is too large to handle, divide and conquer.</t>
   </si>
   <si>
@@ -517,12 +481,6 @@
     <t>lesson_5_end_1</t>
   </si>
   <si>
-    <t>Now it's time to clean up the last remaining blobs, good luck!</t>
-  </si>
-  <si>
-    <t>For example, 9 x 6: multiply 6 by 10 to get 60, and then subtract 6 to get 54.</t>
-  </si>
-  <si>
     <t>mult10_other_title</t>
   </si>
   <si>
@@ -589,9 +547,6 @@
     <t>Commencing mission: Attack on Blob!</t>
   </si>
   <si>
-    <t>With these operators, we can rid of them with ease.</t>
-  </si>
-  <si>
     <t>equal</t>
   </si>
   <si>
@@ -664,7 +619,52 @@
     <t>Unlike multiplication, division is not commutative. So, the order of the numbers cannot be changed.</t>
   </si>
   <si>
-    <t>You have banished all the blobs! Earth is safe!</t>
+    <t>In multiples of three: double the number and then add the original number.</t>
+  </si>
+  <si>
+    <t>When using multiplication, this is a good trick for splitting up a number, then computing each one separately.</t>
+  </si>
+  <si>
+    <t>For the next mission, some blobs must be matched using division. Go ahead and try it out.</t>
+  </si>
+  <si>
+    <t>Before we proceed, let's learn some tricks with multiplication!</t>
+  </si>
+  <si>
+    <t>Rearranging the equation and replacing division with multiplication can help.</t>
+  </si>
+  <si>
+    <t>Now onward to the next mission!</t>
+  </si>
+  <si>
+    <t>You have banished all of the blobs! Earth is safe!</t>
+  </si>
+  <si>
+    <t>With these operators, we can get rid of them with ease.</t>
+  </si>
+  <si>
+    <t>Now it's time to clean up the last remaining blobs. Good luck!</t>
+  </si>
+  <si>
+    <t>With this trick, you only have to remember half of the multiplication table!</t>
+  </si>
+  <si>
+    <t>For example: 2 times 3 and 3 times 2 equal 6.</t>
+  </si>
+  <si>
+    <t>For example, 3 times 6: double 6 to get 12, and then add 6 to get 18.</t>
+  </si>
+  <si>
+    <t>For example, 4 times 6: double 6 to get 12, and then double 12 to get 24.</t>
+  </si>
+  <si>
+    <t>For example, 6 times 7: multiply 7 by 5 to get 35, and then add 7 to get 42.</t>
+  </si>
+  <si>
+    <t>For example, 8 times 4: double 4 to get 8, double 8 to get 16, and finally double 16 to get 32.</t>
+  </si>
+  <si>
+    <t>For example, 9 times 6: multiply 6 by 10 to get 60, and then subtract 6 to get 54.</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1003,7 @@
   <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,31 +1047,31 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1092,18 +1092,18 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1236,66 +1236,66 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B28" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B30" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B33" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="B34" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,90 +1308,90 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="B45" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C46">
         <v>3.5</v>
@@ -1399,10 +1399,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C47">
         <v>3.5</v>
@@ -1410,26 +1410,26 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1442,34 +1442,34 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B54" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1477,7 +1477,7 @@
         <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1485,7 +1485,7 @@
         <v>44</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1501,7 +1501,7 @@
         <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>123</v>
+        <v>209</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1509,7 +1509,7 @@
         <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>208</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1517,7 +1517,7 @@
         <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1530,79 +1530,79 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>210</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>62</v>
+      </c>
+      <c r="B68" t="s">
         <v>64</v>
-      </c>
-      <c r="B68" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
         <v>54</v>
@@ -1610,218 +1610,218 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B78" t="s">
-        <v>126</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B82" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B84" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B85" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B87" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B88" t="s">
-        <v>138</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B89" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B90" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>131</v>
+      </c>
+      <c r="B91" t="s">
         <v>141</v>
-      </c>
-      <c r="B91" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B92" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B93" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="B94" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B95" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="B96" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="B97" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="C99">
         <v>2</v>
@@ -1829,10 +1829,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B100" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C100">
         <v>5</v>
@@ -1840,10 +1840,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="B101" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="C101">
         <v>3</v>
@@ -1851,50 +1851,50 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="B103" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B104" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B105" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B106" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B107" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dumb bonus round to satisfy criteria
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA8E56-265D-4147-99DA-F189D626AF26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F9B843-0174-41BA-8ACE-4DBC79D50491}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
   <si>
     <t>Key</t>
   </si>
@@ -665,6 +665,60 @@
   </si>
   <si>
     <t>For example, 9 times 6: multiply 6 by 10 to get 60, and then subtract 6 to get 54.</t>
+  </si>
+  <si>
+    <t>bonus_round</t>
+  </si>
+  <si>
+    <t>BONUS ROUND</t>
+  </si>
+  <si>
+    <t>commutative</t>
+  </si>
+  <si>
+    <t>associative</t>
+  </si>
+  <si>
+    <t>distributive</t>
+  </si>
+  <si>
+    <t>COMMUTATIVE</t>
+  </si>
+  <si>
+    <t>ASSOCIATIVE</t>
+  </si>
+  <si>
+    <t>DISTRIBUTIVE</t>
+  </si>
+  <si>
+    <t>bonus_instruct</t>
+  </si>
+  <si>
+    <t>Drag the correct numbers on the slots.</t>
+  </si>
+  <si>
+    <t>proceed</t>
+  </si>
+  <si>
+    <t>PROCEED</t>
+  </si>
+  <si>
+    <t>bonus_incorrect</t>
+  </si>
+  <si>
+    <t>INCORRECT!</t>
+  </si>
+  <si>
+    <t>bonus_score_format</t>
+  </si>
+  <si>
+    <t>BONUS SCORE: +{0}</t>
+  </si>
+  <si>
+    <t>bonus_time_expired</t>
+  </si>
+  <si>
+    <t>TIME'S UP!</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,6 +1951,93 @@
         <v>190</v>
       </c>
     </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" t="s">
+        <v>216</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>217</v>
+      </c>
+      <c r="B109" t="s">
+        <v>220</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
+        <v>221</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>219</v>
+      </c>
+      <c r="B111" t="s">
+        <v>222</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>223</v>
+      </c>
+      <c r="B112" t="s">
+        <v>224</v>
+      </c>
+      <c r="C112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>225</v>
+      </c>
+      <c r="B113" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>231</v>
+      </c>
+      <c r="B114" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>227</v>
+      </c>
+      <c r="B115" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>229</v>
+      </c>
+      <c r="B116" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
more bonus round crap, change link clearing to a button
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F9B843-0174-41BA-8ACE-4DBC79D50491}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D13B74F-5C09-4EC7-B28D-9E332B4B8D23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="237">
   <si>
     <t>Key</t>
   </si>
@@ -719,6 +719,18 @@
   </si>
   <si>
     <t>TIME'S UP!</t>
+  </si>
+  <si>
+    <t>division_cap</t>
+  </si>
+  <si>
+    <t>DIVISION</t>
+  </si>
+  <si>
+    <t>link_disconnect_tutorial</t>
+  </si>
+  <si>
+    <t>Press this button to remove all the links.</t>
   </si>
 </sst>
 </file>
@@ -1054,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +1971,7 @@
         <v>216</v>
       </c>
       <c r="C108">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -1997,45 +2009,64 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>233</v>
+      </c>
+      <c r="B112" t="s">
+        <v>234</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>223</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B113" t="s">
         <v>224</v>
       </c>
-      <c r="C112">
+      <c r="C113">
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>225</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>231</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B115" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>227</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>229</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>235</v>
+      </c>
+      <c r="B118" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added ranking based on score
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D13B74F-5C09-4EC7-B28D-9E332B4B8D23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE0C304-08A1-4EC3-B06D-FAF758DAB7A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5085" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="239">
   <si>
     <t>Key</t>
   </si>
@@ -731,6 +731,12 @@
   </si>
   <si>
     <t>Press this button to remove all the links.</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>RANK</t>
   </si>
 </sst>
 </file>
@@ -1066,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+      <selection activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,6 +2075,14 @@
         <v>236</v>
       </c>
     </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>237</v>
+      </c>
+      <c r="B119" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added retry for "C" score, slow down blobs, slightly increase combo duration for the mathematically-challenged.
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A083626-45A5-4AD0-8BB1-993E8FF9F16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DAD5F5-060D-41CA-A583-7B0C69833ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2865" windowWidth="31845" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2865" windowWidth="20220" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="365">
   <si>
     <t>Key</t>
   </si>
@@ -1086,6 +1086,36 @@
   </si>
   <si>
     <t>RANGO</t>
+  </si>
+  <si>
+    <t>newGame</t>
+  </si>
+  <si>
+    <t>NEW GAME</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>CONTINUE</t>
+  </si>
+  <si>
+    <t>NUEVO JUEGO</t>
+  </si>
+  <si>
+    <t>CONTINUAR</t>
+  </si>
+  <si>
+    <t>retry_desc</t>
+  </si>
+  <si>
+    <t>restart</t>
+  </si>
+  <si>
+    <t>It seems you had some trouble with this level. Press RESTART if you want to try again, or CONTINUE to go to the next lesson.</t>
+  </si>
+  <si>
+    <t>RESTART</t>
   </si>
 </sst>
 </file>
@@ -1421,10 +1451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,866 +1527,860 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
+        <v>355</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
+        <v>357</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>156</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>165</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B33" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46">
-        <v>3.5</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47">
-        <v>3.5</v>
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>135</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>85</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>138</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>116</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>133</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>87</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>118</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>43</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>44</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>49</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>50</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>51</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>52</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>53</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>89</v>
-      </c>
-      <c r="B63" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>210</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>60</v>
+        <v>199</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B70" t="s">
-        <v>198</v>
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B71" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>198</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B80" t="s">
-        <v>109</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B84" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B85" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B86" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B88" t="s">
-        <v>213</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B89" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B91" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B92" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B93" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B94" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>214</v>
+        <v>144</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B96" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B97" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B98" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="B99" t="s">
-        <v>192</v>
-      </c>
-      <c r="C99">
-        <v>2</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="B100" t="s">
-        <v>205</v>
-      </c>
-      <c r="C100">
-        <v>5</v>
+        <v>207</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C101">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B102" t="s">
-        <v>180</v>
+        <v>205</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B103" t="s">
-        <v>182</v>
+        <v>194</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B104" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B105" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B106" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="B108" t="s">
-        <v>216</v>
-      </c>
-      <c r="C108">
-        <v>1.5</v>
+        <v>188</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="B109" t="s">
-        <v>220</v>
-      </c>
-      <c r="C109">
-        <v>1</v>
+        <v>190</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B110" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B111" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -2364,10 +2388,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B112" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -2375,75 +2399,113 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B113" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B114" t="s">
-        <v>226</v>
+        <v>234</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B115" t="s">
-        <v>232</v>
+        <v>224</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B116" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B117" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B118" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>229</v>
+      </c>
+      <c r="B119" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>235</v>
+      </c>
+      <c r="B120" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>237</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B121" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>361</v>
+      </c>
+      <c r="B122" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>362</v>
+      </c>
+      <c r="B123" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647008D9-8127-4939-99EE-87A43BAADE43}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,866 +2578,860 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>355</v>
       </c>
       <c r="B7" t="s">
-        <v>244</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>357</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>257</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="B29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B31" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B33" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>282</v>
-      </c>
-      <c r="C46">
-        <v>3.5</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
-        <v>283</v>
-      </c>
-      <c r="C47">
-        <v>3.5</v>
+        <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>282</v>
+      </c>
+      <c r="C48">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" t="s">
+        <v>283</v>
+      </c>
+      <c r="C49">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>135</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>85</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>138</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>47</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>116</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>133</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>87</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>118</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>43</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>44</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>49</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>50</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>51</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>52</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>53</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>298</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>89</v>
-      </c>
-      <c r="B63" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>56</v>
-      </c>
-      <c r="B64" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B68" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B70" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B71" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B75" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B77" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B78" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B80" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B83" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B84" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B85" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B86" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B88" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B89" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B90" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B91" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B92" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B93" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="B94" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B95" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B96" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B97" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B98" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>191</v>
+        <v>150</v>
       </c>
       <c r="B99" t="s">
-        <v>334</v>
-      </c>
-      <c r="C99">
-        <v>2</v>
+        <v>332</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>193</v>
+        <v>152</v>
       </c>
       <c r="B100" t="s">
-        <v>335</v>
-      </c>
-      <c r="C100">
-        <v>5</v>
+        <v>333</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B101" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C101">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="B102" t="s">
-        <v>337</v>
+        <v>335</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B103" t="s">
-        <v>338</v>
+        <v>336</v>
+      </c>
+      <c r="C103">
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B104" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B105" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B106" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B107" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="B108" t="s">
-        <v>343</v>
-      </c>
-      <c r="C108">
-        <v>1.5</v>
+        <v>341</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="B109" t="s">
-        <v>344</v>
-      </c>
-      <c r="C109">
-        <v>1</v>
+        <v>342</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B110" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B111" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C111">
         <v>1</v>
@@ -3383,10 +3439,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B112" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -3394,61 +3450,93 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B113" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="B114" t="s">
-        <v>349</v>
+        <v>347</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B115" t="s">
-        <v>350</v>
+        <v>348</v>
+      </c>
+      <c r="C115">
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B116" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B117" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B118" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>229</v>
+      </c>
+      <c r="B119" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>235</v>
+      </c>
+      <c r="B120" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>237</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B121" t="s">
         <v>354</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slightly increase duration of bonus title for text read, new build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DAD5F5-060D-41CA-A583-7B0C69833ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DE9BD7-027B-4752-A083-3828F0C9C5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2865" windowWidth="20220" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="2865" windowWidth="20220" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -1453,8 +1453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,7 +2383,7 @@
         <v>220</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2394,7 +2394,7 @@
         <v>221</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2405,7 +2405,7 @@
         <v>222</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
         <v>234</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2504,8 +2504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647008D9-8127-4939-99EE-87A43BAADE43}">
   <dimension ref="A1:D123"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3434,7 +3434,7 @@
         <v>344</v>
       </c>
       <c r="C111">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3445,7 +3445,7 @@
         <v>345</v>
       </c>
       <c r="C112">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3456,7 +3456,7 @@
         <v>346</v>
       </c>
       <c r="C113">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3467,7 +3467,7 @@
         <v>347</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>